<commit_message>
change the aspiration criterion
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="285" windowWidth="20355" windowHeight="14595" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="5865" yWindow="285" windowWidth="20355" windowHeight="14595" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="R101" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="78">
   <si>
     <t>Route Number</t>
   </si>
@@ -453,6 +453,21 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>obj</t>
+  </si>
+  <si>
+    <t>m*n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>fre</t>
   </si>
 </sst>
 </file>
@@ -3979,8 +3994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5141,7 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+      <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7419,10 +7434,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK70"/>
+  <dimension ref="A1:AK103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I40" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="U75" sqref="U75"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9614,6 +9629,263 @@
       </c>
       <c r="AB70" s="10">
         <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="84" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <v>1.5</v>
+      </c>
+      <c r="E84">
+        <f>D84*D83</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="85" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <v>1.5</v>
+      </c>
+      <c r="E85">
+        <f>E84*D84</f>
+        <v>3.375</v>
+      </c>
+      <c r="I85">
+        <v>157.01</v>
+      </c>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+    </row>
+    <row r="86" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <v>1.5</v>
+      </c>
+      <c r="E86">
+        <f t="shared" ref="E86:E103" si="0">E85*D85</f>
+        <v>5.0625</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K86" s="10">
+        <v>1685.4749999999999</v>
+      </c>
+      <c r="L86" s="10"/>
+    </row>
+    <row r="87" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>1.5</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="0"/>
+        <v>7.59375</v>
+      </c>
+      <c r="I87">
+        <v>17.009699999999999</v>
+      </c>
+      <c r="J87" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="K87" s="10">
+        <v>1400</v>
+      </c>
+      <c r="L87" s="10">
+        <f>SQRT(K87)</f>
+        <v>37.416573867739416</v>
+      </c>
+    </row>
+    <row r="88" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>1.5</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="0"/>
+        <v>11.390625</v>
+      </c>
+      <c r="I88">
+        <v>281.68</v>
+      </c>
+      <c r="J88" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K88" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L88" s="10">
+        <f>L87*K88*K86</f>
+        <v>945.9704975959213</v>
+      </c>
+      <c r="M88" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <v>1.5</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="0"/>
+        <v>17.0859375</v>
+      </c>
+      <c r="I89">
+        <f>SUM(I85:I88)</f>
+        <v>455.69970000000001</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K89" s="10">
+        <v>2</v>
+      </c>
+      <c r="L89" s="10">
+        <f>L88*K89</f>
+        <v>1891.9409951918426</v>
+      </c>
+    </row>
+    <row r="90" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <v>1.5</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="0"/>
+        <v>25.62890625</v>
+      </c>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+    </row>
+    <row r="91" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <v>1.5</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="0"/>
+        <v>38.443359375</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K91" s="10">
+        <v>2273.7600000000002</v>
+      </c>
+      <c r="L91" s="10">
+        <f>K91+L89</f>
+        <v>4165.7009951918426</v>
+      </c>
+    </row>
+    <row r="92" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>1.5</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="0"/>
+        <v>57.6650390625</v>
+      </c>
+    </row>
+    <row r="93" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>1.5</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="0"/>
+        <v>86.49755859375</v>
+      </c>
+    </row>
+    <row r="94" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <v>1.5</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="0"/>
+        <v>129.746337890625</v>
+      </c>
+    </row>
+    <row r="95" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <v>1.5</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="0"/>
+        <v>194.6195068359375</v>
+      </c>
+    </row>
+    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <v>1.5</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="0"/>
+        <v>291.92926025390625</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <v>1.5</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="0"/>
+        <v>437.89389038085937</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <v>1.5</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="0"/>
+        <v>656.84083557128906</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <v>1.5</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="0"/>
+        <v>985.26125335693359</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <v>1.5</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="0"/>
+        <v>1477.8918800354004</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <v>1.5</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="0"/>
+        <v>2216.8378200531006</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <v>1.5</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="0"/>
+        <v>3325.2567300796509</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <v>1.5</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="0"/>
+        <v>4987.8850951194763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the initial aspiration values, change the attribute initial visited time, diversification factor to 2000
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="285" windowWidth="20355" windowHeight="14595" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="7920" yWindow="1920" windowWidth="20360" windowHeight="14600" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="R101" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Verify" sheetId="8" r:id="rId11"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1311,12 +1311,12 @@
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>1847.21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>3654.77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1451,12 +1451,12 @@
         <v>5.8005100000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="21">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>1846.39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>3580.15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -1633,12 +1633,12 @@
         <v>5.8005100000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="21">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="B29" t="s">
         <v>1</v>
       </c>
@@ -1690,17 +1690,17 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="B30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="B31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11">
       <c r="B33" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>1738.68</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11">
       <c r="B34" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>3584.26</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11">
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11">
       <c r="B36" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11">
       <c r="B38" t="s">
         <v>11</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11">
       <c r="K39">
         <v>1674.43</v>
       </c>
@@ -1864,12 +1864,12 @@
       <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="19.625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="11" t="s">
         <v>32</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
         <v>32</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="11" t="s">
         <v>32</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="11" t="s">
         <v>32</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="11" t="s">
         <v>32</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="11" t="s">
         <v>32</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="11" t="s">
         <v>32</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="11" t="s">
         <v>32</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="11" t="s">
         <v>32</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="11" t="s">
         <v>32</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="11" t="s">
         <v>32</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="11" t="s">
         <v>32</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="F21">
         <f>SUM(F1:F19)</f>
         <v>1650.79864</v>
@@ -2444,15 +2444,15 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="7" width="10.625" customWidth="1"/>
-    <col min="8" max="8" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13">
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13">
       <c r="B2" s="10">
         <v>0</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13">
       <c r="B3" s="10">
         <v>42</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>35.495097567963924</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13">
       <c r="B4" s="10">
         <v>43</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>54.550482706101342</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13">
       <c r="B5" s="10">
         <v>15</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>71.830592595381859</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13">
       <c r="B6" s="10">
         <v>87</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13">
       <c r="B7" s="10">
         <v>57</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13">
       <c r="B8" s="10">
         <v>41</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13">
       <c r="B9" s="10">
         <v>22</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13">
       <c r="B10" s="10">
         <v>74</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13">
       <c r="B11" s="10">
         <v>73</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13">
       <c r="B12" s="10">
         <v>21</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13">
       <c r="B13" s="10">
         <v>26</v>
       </c>
@@ -2717,9 +2717,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:5">
       <c r="C1" t="s">
         <v>70</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2">
         <v>1524.29</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>1519.66</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5">
       <c r="C3">
         <v>0</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4">
         <v>14.094900000000001</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5">
       <c r="C5">
         <v>943.13699999999994</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>781.649</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5">
       <c r="C6">
         <f>SUM(C2:C5)</f>
         <v>2481.5218999999997</v>
@@ -2790,6 +2790,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2801,24 +2806,24 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
-    <col min="8" max="8" width="10.125" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="21">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -2888,7 +2893,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -2905,7 +2910,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -2922,7 +2927,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>1515.96</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>3284.28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -3132,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -3167,7 +3172,7 @@
         <v>4.0275800000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -3196,7 +3201,7 @@
         <v>1519.98</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -3228,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -3242,12 +3247,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -3270,7 +3275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -3293,7 +3298,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -3309,7 +3314,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -3332,7 +3337,7 @@
         <v>1367.66</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -3355,7 +3360,7 @@
         <v>2895.58</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -3378,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -3401,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -3421,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="B31" t="s">
         <v>11</v>
       </c>
@@ -3441,7 +3446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="B32" t="s">
         <v>17</v>
       </c>
@@ -3452,12 +3457,12 @@
         <v>1275.02</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="B35" t="s">
         <v>0</v>
       </c>
@@ -3480,7 +3485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="B36" t="s">
         <v>1</v>
       </c>
@@ -3503,7 +3508,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="B37" t="s">
         <v>2</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -3525,7 +3530,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="B40" t="s">
         <v>4</v>
       </c>
@@ -3548,7 +3553,7 @@
         <v>1038.08</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="B41" t="s">
         <v>5</v>
       </c>
@@ -3571,7 +3576,7 @@
         <v>2431.02</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="B42" t="s">
         <v>6</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="B43" t="s">
         <v>7</v>
       </c>
@@ -3617,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="B44" t="s">
         <v>8</v>
       </c>
@@ -3640,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="B45" t="s">
         <v>11</v>
       </c>
@@ -3663,7 +3668,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="B46" t="s">
         <v>17</v>
       </c>
@@ -3686,12 +3691,12 @@
         <v>1038.08</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="B49" t="s">
         <v>0</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="B50" t="s">
         <v>1</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="B51" t="s">
         <v>2</v>
       </c>
@@ -3727,7 +3732,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="B52" t="s">
         <v>3</v>
       </c>
@@ -3735,7 +3740,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="B54" t="s">
         <v>4</v>
       </c>
@@ -3749,7 +3754,7 @@
         <v>1474.52</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="B55" t="s">
         <v>5</v>
       </c>
@@ -3763,7 +3768,7 @@
         <v>2711.18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="B56" t="s">
         <v>6</v>
       </c>
@@ -3777,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="B57" t="s">
         <v>7</v>
       </c>
@@ -3791,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="B58" t="s">
         <v>8</v>
       </c>
@@ -3805,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="B59" t="s">
         <v>11</v>
       </c>
@@ -3819,7 +3824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -3833,12 +3838,12 @@
         <v>1464.16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -3852,7 +3857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5">
       <c r="B65" t="s">
         <v>1</v>
       </c>
@@ -3866,7 +3871,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5">
       <c r="B66" t="s">
         <v>2</v>
       </c>
@@ -3874,7 +3879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5">
       <c r="B67" t="s">
         <v>3</v>
       </c>
@@ -3882,7 +3887,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5">
       <c r="B69" t="s">
         <v>4</v>
       </c>
@@ -3896,7 +3901,7 @@
         <v>1273.3800000000001</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5">
       <c r="B70" t="s">
         <v>5</v>
       </c>
@@ -3910,7 +3915,7 @@
         <v>2563.73</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5">
       <c r="B71" t="s">
         <v>6</v>
       </c>
@@ -3924,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5">
       <c r="B72" t="s">
         <v>7</v>
       </c>
@@ -3938,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5">
       <c r="B73" t="s">
         <v>8</v>
       </c>
@@ -3952,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5">
       <c r="B74" t="s">
         <v>11</v>
       </c>
@@ -3966,7 +3971,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5">
       <c r="B75" t="s">
         <v>17</v>
       </c>
@@ -3994,24 +3999,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="19" customHeight="1"/>
+    <row r="2" spans="1:3" ht="19" customHeight="1">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19" customHeight="1">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -4019,7 +4024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -4027,7 +4032,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14" customHeight="1">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -4035,7 +4040,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4043,7 +4048,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -4051,7 +4056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -4059,7 +4064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>1726.69</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -4075,7 +4080,7 @@
         <v>3698.27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -4083,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -4091,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -4099,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -4107,7 +4112,7 @@
         <v>1721.19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -4115,12 +4120,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -4165,7 +4170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -4209,7 +4214,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -4227,7 +4232,7 @@
       </c>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -4245,7 +4250,7 @@
       </c>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -4266,7 +4271,7 @@
       </c>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="B24" t="s">
         <v>19</v>
       </c>
@@ -4287,10 +4292,10 @@
       </c>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -4325,7 +4330,7 @@
         <v>1506.24</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="B27" t="s">
         <v>5</v>
       </c>
@@ -4354,7 +4359,7 @@
         <v>3333.1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="B28" t="s">
         <v>6</v>
       </c>
@@ -4389,7 +4394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -4424,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="B30" t="s">
         <v>8</v>
       </c>
@@ -4459,7 +4464,7 @@
         <v>4.0275800000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="B31" t="s">
         <v>14</v>
       </c>
@@ -4492,7 +4497,7 @@
         <v>1481.76</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="B32" t="s">
         <v>22</v>
       </c>
@@ -4510,7 +4515,7 @@
       </c>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="B33" t="s">
         <v>21</v>
       </c>
@@ -4554,10 +4559,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="P34" s="4"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4565,42 +4570,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="B37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="B38" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="B39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19">
       <c r="B41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19">
       <c r="B42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19">
       <c r="B43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19">
       <c r="B44" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -4608,57 +4613,57 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19">
       <c r="B46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19">
       <c r="B47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="B50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="B51" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="B52" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="B55" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="B56" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="B57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="B58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -4666,72 +4671,72 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="B60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="B61" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="B64" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14">
       <c r="B65" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14">
       <c r="B66" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14">
       <c r="B67" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14">
       <c r="B69" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14">
       <c r="B70" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14">
       <c r="B71" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14">
       <c r="B72" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14">
       <c r="B73" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14">
       <c r="B74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14">
       <c r="B75" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -4770,7 +4775,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14">
       <c r="B80" t="s">
         <v>1</v>
       </c>
@@ -4806,7 +4811,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14">
       <c r="B81" t="s">
         <v>2</v>
       </c>
@@ -4825,7 +4830,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14">
       <c r="B82" t="s">
         <v>3</v>
       </c>
@@ -4844,7 +4849,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14">
       <c r="B83" t="s">
         <v>24</v>
       </c>
@@ -4863,7 +4868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14">
       <c r="B84" t="s">
         <v>19</v>
       </c>
@@ -4882,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14">
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -4893,7 +4898,7 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14">
       <c r="B86" t="s">
         <v>23</v>
       </c>
@@ -4929,7 +4934,7 @@
         <v>1310.3399999999999</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14">
       <c r="B87" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +4960,7 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14">
       <c r="B88" t="s">
         <v>6</v>
       </c>
@@ -4991,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14">
       <c r="B89" t="s">
         <v>7</v>
       </c>
@@ -5027,7 +5032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14">
       <c r="B90" t="s">
         <v>8</v>
       </c>
@@ -5060,7 +5065,7 @@
         <v>0.98702500000000004</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14">
       <c r="B91" t="s">
         <v>14</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>1311.67</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:14">
       <c r="B92" t="s">
         <v>21</v>
       </c>
@@ -5144,18 +5149,18 @@
       <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="7" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -5181,7 +5186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -5203,21 +5208,21 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>24</v>
@@ -5236,7 +5241,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -5255,7 +5260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>23</v>
@@ -5283,7 +5288,7 @@
         <v>43.809999999999945</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
@@ -5309,7 +5314,7 @@
         <v>2.6538647928277165E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>7</v>
@@ -5331,7 +5336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -5353,7 +5358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>14</v>
@@ -5375,7 +5380,7 @@
         <v>1672.67</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
         <v>21</v>
@@ -5397,10 +5402,10 @@
         <v>67725</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="4" customFormat="1">
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -5429,7 +5434,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>1</v>
@@ -5454,7 +5459,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>2</v>
@@ -5467,7 +5472,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>3</v>
@@ -5480,7 +5485,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>24</v>
@@ -5499,7 +5504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
@@ -5518,7 +5523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>23</v>
@@ -5549,7 +5554,7 @@
         <v>1787.96</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
         <v>6</v>
@@ -5578,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
         <v>7</v>
@@ -5603,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
         <v>8</v>
@@ -5628,7 +5633,7 @@
         <v>17.194900000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
         <v>14</v>
@@ -5653,7 +5658,7 @@
         <v>1484.83</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>21</v>
@@ -5678,10 +5683,10 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="4" customFormat="1">
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
@@ -5731,7 +5736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
         <v>1</v>
@@ -5777,7 +5782,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>2</v>
@@ -5787,7 +5792,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
         <v>3</v>
@@ -5797,7 +5802,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>24</v>
@@ -5825,7 +5830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
         <v>19</v>
@@ -5853,7 +5858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
         <v>23</v>
@@ -5901,7 +5906,7 @@
         <v>2516.29</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>6</v>
@@ -5947,7 +5952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>7</v>
@@ -5993,7 +5998,7 @@
         <v>1067.71</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
         <v>8</v>
@@ -6039,7 +6044,7 @@
         <v>4376.72</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
         <v>14</v>
@@ -6085,7 +6090,7 @@
         <v>1885.94</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
         <v>21</v>
@@ -6131,10 +6136,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" s="4" customFormat="1">
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23">
       <c r="A41" s="5" t="s">
         <v>16</v>
       </c>
@@ -6190,7 +6195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
         <v>1</v>
@@ -6242,7 +6247,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>2</v>
@@ -6252,7 +6257,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>3</v>
@@ -6262,7 +6267,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="s">
         <v>24</v>
@@ -6311,7 +6316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
         <v>19</v>
@@ -6360,7 +6365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
         <v>23</v>
@@ -6418,7 +6423,7 @@
         <v>1112.42</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
         <v>6</v>
@@ -6474,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23">
       <c r="A49" s="5"/>
       <c r="B49" s="5" t="s">
         <v>7</v>
@@ -6526,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
         <v>8</v>
@@ -6578,7 +6583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
         <v>14</v>
@@ -6630,7 +6635,7 @@
         <v>1107.83</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>21</v>
@@ -6682,10 +6687,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" s="4" customFormat="1">
       <c r="C53" s="6"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23">
       <c r="A54" s="5" t="s">
         <v>15</v>
       </c>
@@ -6711,7 +6716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
         <v>1</v>
@@ -6733,21 +6738,21 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C56" s="7"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
         <v>24</v>
@@ -6769,7 +6774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
         <v>19</v>
@@ -6791,7 +6796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="s">
         <v>23</v>
@@ -6819,7 +6824,7 @@
         <v>1495.02</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
         <v>6</v>
@@ -6845,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
         <v>7</v>
@@ -6867,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
         <v>8</v>
@@ -6889,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23">
       <c r="A64" s="5"/>
       <c r="B64" s="5" t="s">
         <v>14</v>
@@ -6911,7 +6916,7 @@
         <v>1473.62</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
         <v>21</v>
@@ -6933,10 +6938,10 @@
         <v>452</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" s="4" customFormat="1">
       <c r="C66" s="6"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19">
       <c r="B68" t="s">
         <v>1</v>
       </c>
@@ -7030,7 +7035,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19">
       <c r="B69" t="s">
         <v>2</v>
       </c>
@@ -7038,7 +7043,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19">
       <c r="B70" t="s">
         <v>3</v>
       </c>
@@ -7046,7 +7051,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19">
       <c r="B71" t="s">
         <v>24</v>
       </c>
@@ -7084,7 +7089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19">
       <c r="B72" t="s">
         <v>19</v>
       </c>
@@ -7122,7 +7127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19">
       <c r="B73" t="s">
         <v>27</v>
       </c>
@@ -7145,7 +7150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19">
       <c r="B74" t="s">
         <v>23</v>
       </c>
@@ -7196,7 +7201,7 @@
         <v>1460.18</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19">
       <c r="B75" t="s">
         <v>6</v>
       </c>
@@ -7244,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19">
       <c r="B76" t="s">
         <v>7</v>
       </c>
@@ -7288,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19">
       <c r="B77" t="s">
         <v>8</v>
       </c>
@@ -7332,7 +7337,7 @@
         <v>21.2257</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19">
       <c r="B78" t="s">
         <v>14</v>
       </c>
@@ -7376,7 +7381,7 @@
         <v>1514.41</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19">
       <c r="B79" t="s">
         <v>21</v>
       </c>
@@ -7436,25 +7441,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView topLeftCell="AE35" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="U65" sqref="U65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="7" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="31" max="31" width="21" customWidth="1"/>
     <col min="32" max="32" width="17" customWidth="1"/>
-    <col min="33" max="33" width="17.625" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -7474,7 +7479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
@@ -7490,7 +7495,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>41</v>
@@ -7506,7 +7511,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>27</v>
@@ -7516,7 +7521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -7534,7 +7539,7 @@
         <v>1921.6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
@@ -7551,7 +7556,7 @@
       </c>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>7</v>
@@ -7567,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
@@ -7583,7 +7588,7 @@
         <v>42.352200000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
@@ -7599,7 +7604,7 @@
         <v>1696.58</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>21</v>
@@ -7615,10 +7620,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="4" customFormat="1">
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -7629,42 +7634,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>23</v>
@@ -7673,7 +7678,7 @@
         <v>1488.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>6</v>
@@ -7681,38 +7686,38 @@
       <c r="C20" s="7"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="4" customFormat="1">
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -7723,42 +7728,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>23</v>
@@ -7767,45 +7772,45 @@
         <v>1299.78</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" s="4" customFormat="1">
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
@@ -7858,7 +7863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="s">
         <v>1</v>
@@ -7907,7 +7912,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
         <v>39</v>
@@ -7956,7 +7961,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
         <v>27</v>
@@ -7966,7 +7971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>23</v>
@@ -8017,7 +8022,7 @@
         <v>998.14</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>6</v>
@@ -8066,7 +8071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="s">
         <v>7</v>
@@ -8115,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
         <v>8</v>
@@ -8164,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
         <v>14</v>
@@ -8213,7 +8218,7 @@
         <v>998.14</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
         <v>21</v>
@@ -8244,10 +8249,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37" s="4" customFormat="1">
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37">
       <c r="A50" s="5" t="s">
         <v>15</v>
       </c>
@@ -8297,7 +8302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
         <v>1</v>
@@ -8343,7 +8348,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>39</v>
@@ -8389,7 +8394,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
         <v>27</v>
@@ -8402,7 +8407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>23</v>
@@ -8450,7 +8455,7 @@
         <v>1422.28</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
         <v>6</v>
@@ -8496,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
         <v>7</v>
@@ -8542,7 +8547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -8588,7 +8593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
         <v>14</v>
@@ -8634,7 +8639,7 @@
         <v>1418.73</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
         <v>21</v>
@@ -8662,10 +8667,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37" s="4" customFormat="1">
       <c r="C60" s="6"/>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -8766,7 +8771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37">
       <c r="B62" t="s">
         <v>1</v>
       </c>
@@ -8867,7 +8872,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37">
       <c r="B63" t="s">
         <v>39</v>
       </c>
@@ -8956,7 +8961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37">
       <c r="B64" t="s">
         <v>27</v>
       </c>
@@ -9048,7 +9053,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:37">
       <c r="B65" t="s">
         <v>23</v>
       </c>
@@ -9152,7 +9157,7 @@
         <v>1530.58</v>
       </c>
     </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:37">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -9254,7 +9259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:37">
       <c r="B67" t="s">
         <v>7</v>
       </c>
@@ -9355,7 +9360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:37">
       <c r="B68" t="s">
         <v>8</v>
       </c>
@@ -9456,7 +9461,7 @@
         <v>10.484</v>
       </c>
     </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:37">
       <c r="B69" t="s">
         <v>14</v>
       </c>
@@ -9557,7 +9562,7 @@
         <v>1446.47</v>
       </c>
     </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:37">
       <c r="B70" t="s">
         <v>21</v>
       </c>
@@ -9631,12 +9636,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:13">
       <c r="D83">
         <v>1.5</v>
       </c>
     </row>
-    <row r="84" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:13">
       <c r="D84">
         <v>1.5</v>
       </c>
@@ -9645,7 +9650,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="85" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:13">
       <c r="D85">
         <v>1.5</v>
       </c>
@@ -9660,7 +9665,7 @@
       <c r="K85" s="10"/>
       <c r="L85" s="10"/>
     </row>
-    <row r="86" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:13">
       <c r="D86">
         <v>1.5</v>
       </c>
@@ -9679,7 +9684,7 @@
       </c>
       <c r="L86" s="10"/>
     </row>
-    <row r="87" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:13">
       <c r="D87">
         <v>1.5</v>
       </c>
@@ -9701,7 +9706,7 @@
         <v>37.416573867739416</v>
       </c>
     </row>
-    <row r="88" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:13">
       <c r="D88">
         <v>1.5</v>
       </c>
@@ -9726,7 +9731,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="89" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:13">
       <c r="D89">
         <v>1.5</v>
       </c>
@@ -9749,7 +9754,7 @@
         <v>1891.9409951918426</v>
       </c>
     </row>
-    <row r="90" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:13">
       <c r="D90">
         <v>1.5</v>
       </c>
@@ -9761,7 +9766,7 @@
       <c r="K90" s="10"/>
       <c r="L90" s="10"/>
     </row>
-    <row r="91" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:13">
       <c r="D91">
         <v>1.5</v>
       </c>
@@ -9780,7 +9785,7 @@
         <v>4165.7009951918426</v>
       </c>
     </row>
-    <row r="92" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:13">
       <c r="D92">
         <v>1.5</v>
       </c>
@@ -9789,7 +9794,7 @@
         <v>57.6650390625</v>
       </c>
     </row>
-    <row r="93" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:13">
       <c r="D93">
         <v>1.5</v>
       </c>
@@ -9798,7 +9803,7 @@
         <v>86.49755859375</v>
       </c>
     </row>
-    <row r="94" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:13">
       <c r="D94">
         <v>1.5</v>
       </c>
@@ -9807,7 +9812,7 @@
         <v>129.746337890625</v>
       </c>
     </row>
-    <row r="95" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:13">
       <c r="D95">
         <v>1.5</v>
       </c>
@@ -9816,7 +9821,7 @@
         <v>194.6195068359375</v>
       </c>
     </row>
-    <row r="96" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:13">
       <c r="D96">
         <v>1.5</v>
       </c>
@@ -9825,16 +9830,16 @@
         <v>291.92926025390625</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:5">
       <c r="D97">
         <v>1.5</v>
       </c>
       <c r="E97">
         <f t="shared" si="0"/>
-        <v>437.89389038085937</v>
-      </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+        <v>437.89389038085938</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5">
       <c r="D98">
         <v>1.5</v>
       </c>
@@ -9843,7 +9848,7 @@
         <v>656.84083557128906</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:5">
       <c r="D99">
         <v>1.5</v>
       </c>
@@ -9852,7 +9857,7 @@
         <v>985.26125335693359</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:5">
       <c r="D100">
         <v>1.5</v>
       </c>
@@ -9861,7 +9866,7 @@
         <v>1477.8918800354004</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:5">
       <c r="D101">
         <v>1.5</v>
       </c>
@@ -9870,7 +9875,7 @@
         <v>2216.8378200531006</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:5">
       <c r="D102">
         <v>1.5</v>
       </c>
@@ -9879,7 +9884,7 @@
         <v>3325.2567300796509</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:5">
       <c r="D103">
         <v>1.5</v>
       </c>
@@ -9903,23 +9908,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -9948,7 +9953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -9972,7 +9977,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="C4" t="s">
         <v>39</v>
       </c>
@@ -9996,7 +10001,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -10020,7 +10025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="C6" t="s">
         <v>23</v>
       </c>
@@ -10029,35 +10034,35 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11">
         <v>200</v>
       </c>
@@ -10067,101 +10072,101 @@
       <c r="D11" s="8"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="C13" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10">
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6">
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6">
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6">
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6">
       <c r="E20" s="13"/>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6">
       <c r="C22" t="s">
         <v>57</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6">
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6">
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6">
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6">
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6">
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6">
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6">
       <c r="C30" t="s">
         <v>58</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6">
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6">
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10">
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10">
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:10">
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10">
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10">
       <c r="C38" t="s">
         <v>68</v>
       </c>
@@ -10182,7 +10187,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10">
       <c r="D39" s="8">
         <v>12</v>
       </c>
@@ -10202,7 +10207,7 @@
         <v>1361.99</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10">
       <c r="D40" s="8"/>
       <c r="E40" s="13">
         <v>0</v>
@@ -10220,7 +10225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10">
       <c r="D41" s="8"/>
       <c r="E41" s="13">
         <v>0</v>
@@ -10238,7 +10243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:10">
       <c r="D42" s="8"/>
       <c r="E42" s="13">
         <v>0</v>
@@ -10256,7 +10261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:10">
       <c r="D43" s="8">
         <v>1253.23</v>
       </c>
@@ -10276,14 +10281,14 @@
         <v>1321.8</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:10">
       <c r="D44" s="8"/>
       <c r="E44" s="13">
         <v>18</v>
       </c>
       <c r="F44" s="13"/>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:10">
       <c r="C46" t="s">
         <v>69</v>
       </c>
@@ -10303,7 +10308,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:10">
       <c r="F47" s="13">
         <v>1460.97</v>
       </c>
@@ -10320,7 +10325,7 @@
         <v>1309.68</v>
       </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:10">
       <c r="F48" s="13">
         <v>0</v>
       </c>
@@ -10337,7 +10342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:10">
       <c r="F49" s="13">
         <v>0</v>
       </c>
@@ -10354,7 +10359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:10">
       <c r="F50" s="13">
         <v>0</v>
       </c>
@@ -10371,7 +10376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:10">
       <c r="F51" s="13">
         <v>1348.32</v>
       </c>
@@ -10390,6 +10395,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10401,22 +10411,22 @@
       <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.125" customWidth="1"/>
-    <col min="2" max="2" width="29.875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="7" style="8" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="31" max="31" width="21" customWidth="1"/>
     <col min="32" max="32" width="17" customWidth="1"/>
-    <col min="33" max="33" width="17.625" customWidth="1"/>
+    <col min="33" max="33" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -10427,28 +10437,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>23</v>
@@ -10457,7 +10467,7 @@
         <v>1650.8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
         <v>6</v>
@@ -10465,38 +10475,38 @@
       <c r="C7" s="7"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="4" customFormat="1">
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -10507,42 +10517,42 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>23</v>
@@ -10551,7 +10561,7 @@
         <v>1488.1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>6</v>
@@ -10559,38 +10569,38 @@
       <c r="C20" s="7"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="4" customFormat="1">
       <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
         <v>12</v>
       </c>
@@ -10601,42 +10611,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>23</v>
@@ -10645,45 +10655,45 @@
         <v>1299.78</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="4" customFormat="1">
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
         <v>16</v>
       </c>
@@ -10694,28 +10704,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="5"/>
       <c r="B40" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
         <v>23</v>
@@ -10724,45 +10734,45 @@
         <v>984</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="7"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="7"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="7"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C48" s="7"/>
     </row>
-    <row r="49" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" s="4" customFormat="1">
       <c r="C49" s="6"/>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33">
       <c r="A50" s="5" t="s">
         <v>15</v>
       </c>
@@ -10776,7 +10786,7 @@
         <v>1435.13</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
         <v>1</v>
@@ -10786,7 +10796,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>39</v>
@@ -10796,7 +10806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
         <v>27</v>
@@ -10806,7 +10816,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>23</v>
@@ -10818,7 +10828,7 @@
         <v>1435.13</v>
       </c>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
         <v>6</v>
@@ -10828,7 +10838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
         <v>7</v>
@@ -10838,7 +10848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>8</v>
@@ -10848,7 +10858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
         <v>14</v>
@@ -10858,17 +10868,17 @@
         <v>1430.34</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C59" s="7"/>
     </row>
-    <row r="60" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" s="4" customFormat="1">
       <c r="C60" s="6"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -10930,7 +10940,7 @@
       <c r="AF61" s="10"/>
       <c r="AG61" s="10"/>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33">
       <c r="B62" t="s">
         <v>1</v>
       </c>
@@ -10969,7 +10979,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33">
       <c r="B63" t="s">
         <v>39</v>
       </c>
@@ -11008,7 +11018,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33">
       <c r="B64" t="s">
         <v>27</v>
       </c>
@@ -11038,7 +11048,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:19">
       <c r="B65" t="s">
         <v>23</v>
       </c>
@@ -11083,7 +11093,7 @@
         <v>1290.1300000000001</v>
       </c>
     </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:19">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -11122,7 +11132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:19">
       <c r="B67" t="s">
         <v>7</v>
       </c>
@@ -11161,7 +11171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:19">
       <c r="B68" t="s">
         <v>8</v>
       </c>
@@ -11200,7 +11210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:19">
       <c r="B69" t="s">
         <v>14</v>
       </c>
@@ -11236,7 +11246,7 @@
         <v>1275.05</v>
       </c>
     </row>
-    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:19">
       <c r="B70" t="s">
         <v>21</v>
       </c>
@@ -11276,25 +11286,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J44"/>
+  <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="3" max="3" width="27.625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14">
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="6"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -11322,8 +11332,11 @@
       <c r="J2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -11346,8 +11359,11 @@
       <c r="J3">
         <v>40000</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="C4" t="s">
         <v>39</v>
       </c>
@@ -11371,7 +11387,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -11395,7 +11411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="C6" t="s">
         <v>23</v>
       </c>
@@ -11420,8 +11436,11 @@
       <c r="J6">
         <v>1294.24</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1285.26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -11445,7 +11464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="C8" t="s">
         <v>7</v>
       </c>
@@ -11469,7 +11488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -11493,7 +11512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -11517,7 +11536,7 @@
         <v>1288.25</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14">
       <c r="B11">
         <v>200</v>
       </c>
@@ -11529,7 +11548,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="C13" t="s">
         <v>56</v>
       </c>
@@ -11543,7 +11562,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="E14" s="13">
         <v>38</v>
       </c>
@@ -11554,7 +11573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="E15" s="13">
         <v>1307.4100000000001</v>
       </c>
@@ -11565,7 +11584,7 @@
         <v>1307.4100000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="E16" s="13">
         <v>0</v>
       </c>
@@ -11576,7 +11595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="E17" s="13">
         <v>0</v>
       </c>
@@ -11587,7 +11606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="E18" s="13">
         <v>0</v>
       </c>
@@ -11598,7 +11617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="E19" s="13">
         <v>1307.4100000000001</v>
       </c>
@@ -11609,12 +11628,12 @@
         <v>1294.54</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="E20" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" t="s">
         <v>57</v>
       </c>
@@ -11625,7 +11644,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="E23" s="13">
         <v>38</v>
       </c>
@@ -11633,7 +11652,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="E24" s="13">
         <v>1344.14</v>
       </c>
@@ -11641,7 +11660,7 @@
         <v>1344.14</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="E25" s="13">
         <v>0</v>
       </c>
@@ -11649,7 +11668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="E26" s="13">
         <v>0</v>
       </c>
@@ -11657,7 +11676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="E27" s="13">
         <v>0</v>
       </c>
@@ -11665,7 +11684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7">
       <c r="E28" s="13">
         <v>1326.67</v>
       </c>
@@ -11673,7 +11692,7 @@
         <v>1313.28</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7">
       <c r="C30" t="s">
         <v>58</v>
       </c>
@@ -11687,7 +11706,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7">
       <c r="E31" s="13">
         <v>38</v>
       </c>
@@ -11698,7 +11717,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7">
       <c r="E32" s="13">
         <v>1386.85</v>
       </c>
@@ -11709,7 +11728,7 @@
         <v>1302.8499999999999</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7">
       <c r="E33" s="13">
         <v>0</v>
       </c>
@@ -11720,7 +11739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7">
       <c r="E34" s="13">
         <v>0</v>
       </c>
@@ -11731,7 +11750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7">
       <c r="E35" s="13">
         <v>0</v>
       </c>
@@ -11742,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7">
       <c r="E36" s="13">
         <v>1314.01</v>
       </c>
@@ -11753,7 +11772,7 @@
         <v>1302.83</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7">
       <c r="C38" t="s">
         <v>59</v>
       </c>
@@ -11764,7 +11783,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7">
       <c r="E39" s="13">
         <v>1436.94</v>
       </c>
@@ -11772,7 +11791,7 @@
         <v>1320.59</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7">
       <c r="E40" s="13">
         <v>0</v>
       </c>
@@ -11780,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7">
       <c r="E41" s="13">
         <v>0</v>
       </c>
@@ -11788,7 +11807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7">
       <c r="E42" s="13">
         <v>3.3520400000000001</v>
       </c>
@@ -11796,7 +11815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7">
       <c r="E43" s="13">
         <v>1363.56</v>
       </c>
@@ -11804,7 +11823,7 @@
         <v>1310.69</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7">
       <c r="E44" s="13">
         <v>16</v>
       </c>
@@ -11827,23 +11846,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="8.25" customWidth="1"/>
-    <col min="3" max="3" width="7.25" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="8.25" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" customWidth="1"/>
     <col min="8" max="8" width="7.5" customWidth="1"/>
-    <col min="9" max="9" width="9.25" customWidth="1"/>
-    <col min="10" max="10" width="8.375" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" s="31" t="s">
         <v>60</v>
       </c>
@@ -11862,7 +11881,7 @@
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="32"/>
       <c r="C3" s="14" t="s">
         <v>64</v>
@@ -11889,7 +11908,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="18" t="s">
         <v>25</v>
       </c>
@@ -11920,7 +11939,7 @@
         <v>1.9748000969226987E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" s="23" t="s">
         <v>13</v>
       </c>
@@ -11951,7 +11970,7 @@
         <v>1.4589073314965418E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
@@ -11981,7 +12000,7 @@
         <v>5.5640185262121236E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
@@ -12012,7 +12031,7 @@
         <v>1.3861788617886166E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" s="23" t="s">
         <v>15</v>
       </c>
@@ -12043,7 +12062,7 @@
         <v>1.9853170770672023E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
@@ -12083,5 +12102,10 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
check calculation, no mistake found; check parameter values, found algorithm are easiliy stuck in some point
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="1920" windowWidth="20360" windowHeight="14600" tabRatio="500" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="25600" windowHeight="7440" tabRatio="500" firstSheet="5" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="R101" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="BestResult" sheetId="6" r:id="rId10"/>
     <sheet name="Verify" sheetId="8" r:id="rId11"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -234,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="88">
   <si>
     <t>Route Number</t>
   </si>
@@ -469,6 +470,36 @@
   <si>
     <t>fre</t>
   </si>
+  <si>
+    <t>Ori Id</t>
+  </si>
+  <si>
+    <t>Solomon Id</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Ser T</t>
+  </si>
+  <si>
+    <t>Arrive T</t>
+  </si>
+  <si>
+    <t>Ser Star</t>
+  </si>
+  <si>
+    <t>Ser Com</t>
+  </si>
+  <si>
+    <t>Lateness</t>
+  </si>
 </sst>
 </file>
 
@@ -695,7 +726,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -767,6 +798,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -882,7 +917,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="93">
     <cellStyle name="Bad" xfId="27" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -927,6 +962,8 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="70" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -971,6 +1008,8 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1451,7 +1490,7 @@
         <v>5.8005100000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21">
+    <row r="13" spans="1:8" ht="20">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1633,7 +1672,7 @@
         <v>5.8005100000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="21">
+    <row r="26" spans="1:11" ht="20">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -2798,6 +2837,267 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="B4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>55</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <f>SQRT((D4-D3)^2+(E4-E3)^2)</f>
+        <v>25.495097567963924</v>
+      </c>
+      <c r="L4">
+        <f>K4</f>
+        <v>25.495097567963924</v>
+      </c>
+      <c r="M4">
+        <f>L4</f>
+        <v>25.495097567963924</v>
+      </c>
+      <c r="N4">
+        <f>M4+10</f>
+        <v>35.495097567963924</v>
+      </c>
+      <c r="O4">
+        <f>M4-H4</f>
+        <v>-29.504902432036076</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="B5">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>122</v>
+      </c>
+      <c r="H5">
+        <v>152</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K7" si="0">SQRT((D5-D4)^2+(E5-E4)^2)</f>
+        <v>9.0553851381374173</v>
+      </c>
+      <c r="L5">
+        <f>N4+K5</f>
+        <v>44.550482706101342</v>
+      </c>
+      <c r="M5">
+        <f>G5</f>
+        <v>122</v>
+      </c>
+      <c r="N5">
+        <f>132</f>
+        <v>132</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O6" si="1">M5-H5</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>51</v>
+      </c>
+      <c r="H6">
+        <v>81</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>7.2801098892805181</v>
+      </c>
+      <c r="L6">
+        <f>K6+N5</f>
+        <v>139.28010988928051</v>
+      </c>
+      <c r="M6">
+        <f>L6</f>
+        <v>139.28010988928051</v>
+      </c>
+      <c r="N6">
+        <f>M6+10</f>
+        <v>149.28010988928051</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>58.28010988928051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>230</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>30.413812651491099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="K9">
+        <f>SUM(K4:K7)</f>
+        <v>72.244405246872958</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O75"/>
@@ -2813,7 +3113,7 @@
     <col min="8" max="8" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="21">
+    <row r="2" spans="1:15" ht="20">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -11288,7 +11588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
implement the tabu feature for the 2-opt operator
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="0" windowWidth="25605" windowHeight="7440" tabRatio="500" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="1245" yWindow="0" windowWidth="25605" windowHeight="7440" tabRatio="500" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="R101" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Verify" sheetId="8" r:id="rId11"/>
     <sheet name="Sheet2" sheetId="14" r:id="rId12"/>
     <sheet name="SolutionNew" sheetId="15" r:id="rId13"/>
+    <sheet name="SensitivityAna" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -234,8 +235,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Xie F.</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xie F.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tabu on 2-opt</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="93">
   <si>
     <t>Route Number</t>
   </si>
@@ -494,14 +529,42 @@
   <si>
     <t>Tabu Length</t>
   </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>No Feasible</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>TabuLength</t>
+  </si>
+  <si>
+    <t>IteratrionNum</t>
+  </si>
+  <si>
+    <t>ParameterUpper</t>
+  </si>
+  <si>
+    <t>VehicleNum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -591,8 +654,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,6 +719,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -720,112 +849,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="27"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="27"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,10 +967,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="70" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="70" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,7 +985,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -895,10 +1027,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -910,8 +1042,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="27" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="27" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="94" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="94" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="95" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="93" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="96">
+    <cellStyle name="20% - Accent1" xfId="93" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="94" builtinId="34"/>
+    <cellStyle name="Accent3" xfId="95" builtinId="37"/>
     <cellStyle name="Bad" xfId="27" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3004,11 +3160,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3024,6 +3180,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="6"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3033,6 +3190,12 @@
         <v>0</v>
       </c>
       <c r="C2" s="7">
+        <v>19</v>
+      </c>
+      <c r="D2" s="10">
+        <v>19</v>
+      </c>
+      <c r="E2">
         <v>19</v>
       </c>
     </row>
@@ -3042,827 +3205,883 @@
         <v>1</v>
       </c>
       <c r="C3" s="7"/>
+      <c r="D3" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E3">
+        <v>40000</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7"/>
+      <c r="D4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C5" s="7"/>
+      <c r="D5" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="E5">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7">
         <v>1650.8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C7" s="7"/>
+      <c r="D7" s="10"/>
+      <c r="E7">
+        <v>15</v>
+      </c>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C8" s="7"/>
+      <c r="D8" s="10">
+        <v>1685.89</v>
+      </c>
+      <c r="E8">
+        <v>1655.99</v>
+      </c>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="7"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
         <v>17</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D15" s="10">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="10">
-        <v>0.5</v>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="10">
-        <v>1.4999999999999999E-2</v>
+      <c r="D16" s="10"/>
+      <c r="E16">
+        <v>30000</v>
+      </c>
+      <c r="F16">
+        <v>40000</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="10">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
+      </c>
+      <c r="F17">
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="10">
-        <v>30</v>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1488.1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="10">
-        <v>1522.01</v>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="10">
-        <v>0</v>
-      </c>
-      <c r="J20" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1488.1</v>
+      </c>
       <c r="D21" s="10">
-        <v>0</v>
+        <v>1522.01</v>
+      </c>
+      <c r="E21">
+        <v>1557.79</v>
+      </c>
+      <c r="F21">
+        <v>1516.93</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="10">
         <v>0</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="B28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="7"/>
+      <c r="D28" s="10">
+        <v>13</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C30" s="7"/>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="C31" s="7"/>
+      <c r="D31">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1299.78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1299.78</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="C39" s="7"/>
+    </row>
+    <row r="40" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="7">
+      <c r="B41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>10000</v>
+      </c>
+      <c r="E42">
+        <v>20000</v>
+      </c>
+      <c r="F42">
+        <v>30000</v>
+      </c>
+      <c r="G42">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="7">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43">
+        <v>0.5</v>
+      </c>
+      <c r="E43">
+        <v>0.5</v>
+      </c>
+      <c r="F43">
+        <v>0.5</v>
+      </c>
+      <c r="G43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C45" s="7">
+        <v>984</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <v>15</v>
+      </c>
+      <c r="G46">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>1067.73</v>
+      </c>
+      <c r="E47">
+        <v>1067.73</v>
+      </c>
+      <c r="F47">
+        <v>1061.68</v>
+      </c>
+      <c r="G47">
+        <v>1061.68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C51" s="7"/>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C52" s="7"/>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+    <row r="53" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B54" s="5" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C54" s="7">
-        <v>1377.11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>14</v>
+      </c>
+      <c r="E54">
+        <v>14</v>
+      </c>
+      <c r="F54">
+        <v>14</v>
+      </c>
+      <c r="G54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>10000</v>
+      </c>
+      <c r="E55">
+        <v>20000</v>
+      </c>
+      <c r="F55">
+        <v>30000</v>
+      </c>
+      <c r="G55">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>0.5</v>
+      </c>
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="F56">
+        <v>0.5</v>
+      </c>
+      <c r="G56">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E57">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F57">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G57">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="7"/>
+      <c r="D59">
+        <v>15</v>
+      </c>
+      <c r="E59">
+        <v>15</v>
+      </c>
+      <c r="F59">
+        <v>15</v>
+      </c>
+      <c r="G59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="7">
+        <v>1377.11</v>
+      </c>
+      <c r="D60">
+        <v>1413.08</v>
+      </c>
+      <c r="E60">
+        <v>1410.37</v>
+      </c>
+      <c r="F60">
+        <v>1410.37</v>
+      </c>
+      <c r="G60">
+        <v>1410.37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="6"/>
-    </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="6"/>
+    </row>
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>18</v>
       </c>
-      <c r="B61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="8">
+      <c r="B67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="8">
         <v>12</v>
       </c>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
-      <c r="Q61" s="10"/>
-      <c r="R61" s="10"/>
-      <c r="S61" s="10"/>
-      <c r="T61" s="10"/>
-      <c r="U61" s="10"/>
-      <c r="V61" s="10">
+      <c r="D67" s="10">
         <v>12</v>
       </c>
-      <c r="W61" s="10">
+      <c r="E67" s="10">
         <v>12</v>
       </c>
-      <c r="X61" s="10">
+      <c r="F67" s="10">
         <v>12</v>
       </c>
-      <c r="Y61" s="10">
+      <c r="G67" s="10">
         <v>12</v>
       </c>
-      <c r="Z61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AA61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AB61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AC61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AE61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AF61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AG61" s="10">
-        <v>12</v>
-      </c>
-      <c r="AI61" s="10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
-      <c r="O62" s="10"/>
-      <c r="P62" s="10"/>
-      <c r="Q62" s="10"/>
-      <c r="R62" s="10"/>
-      <c r="S62" s="10"/>
-      <c r="T62" s="10"/>
-      <c r="U62" s="10"/>
-      <c r="V62" s="10">
-        <v>10000</v>
-      </c>
-      <c r="W62" s="10">
-        <v>20000</v>
-      </c>
-      <c r="X62" s="10">
-        <v>30000</v>
-      </c>
-      <c r="Y62" s="10">
-        <v>20000</v>
-      </c>
-      <c r="Z62" s="10">
-        <v>50000</v>
-      </c>
-      <c r="AA62" s="10">
-        <v>10000</v>
-      </c>
-      <c r="AB62" s="10">
-        <v>5325</v>
-      </c>
-      <c r="AC62" s="10">
-        <v>1000</v>
-      </c>
-      <c r="AE62" s="10">
-        <v>50000</v>
-      </c>
-      <c r="AF62" s="10">
-        <v>50000</v>
-      </c>
-      <c r="AG62" s="10">
-        <v>40000</v>
-      </c>
-      <c r="AI62" s="10">
-        <v>1</v>
-      </c>
-      <c r="AJ62" s="10">
-        <v>10</v>
-      </c>
-      <c r="AK62" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>39</v>
-      </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="10"/>
-      <c r="P63" s="10"/>
-      <c r="Q63" s="10"/>
-      <c r="R63" s="10"/>
-      <c r="S63" s="10"/>
-      <c r="T63" s="10"/>
-      <c r="U63" s="10"/>
-      <c r="V63" s="10">
-        <v>20</v>
-      </c>
-      <c r="W63" s="10">
-        <v>20</v>
-      </c>
-      <c r="X63" s="10">
-        <v>20</v>
-      </c>
-      <c r="Y63" s="10"/>
-      <c r="Z63" s="10"/>
-      <c r="AA63" s="10"/>
-      <c r="AB63" s="10">
-        <v>31</v>
-      </c>
-      <c r="AC63">
-        <v>53</v>
-      </c>
-      <c r="AE63" s="10">
-        <v>38</v>
-      </c>
-      <c r="AF63" s="10">
-        <v>39</v>
-      </c>
-      <c r="AG63" s="10">
-        <v>38</v>
-      </c>
-      <c r="AI63" s="10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>27</v>
-      </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
-      <c r="V64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="W64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="X64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA64" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC64" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE64" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF64" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG64" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>23</v>
-      </c>
-      <c r="C65" s="8">
-        <v>1253.23</v>
-      </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="10"/>
-      <c r="N65" s="10"/>
-      <c r="O65" s="10"/>
-      <c r="P65" s="12"/>
-      <c r="Q65" s="10"/>
-      <c r="R65" s="10"/>
-      <c r="S65" s="10"/>
-      <c r="T65" s="10"/>
-      <c r="U65" s="12"/>
-      <c r="V65" s="12">
-        <v>1286.48</v>
-      </c>
-      <c r="W65" s="10">
-        <v>1286.48</v>
-      </c>
-      <c r="X65" s="10">
-        <v>1286.48</v>
-      </c>
-      <c r="Y65" s="10">
-        <v>1314.56</v>
-      </c>
-      <c r="Z65" s="10">
-        <v>1314.56</v>
-      </c>
-      <c r="AA65" s="10">
-        <v>1433.36</v>
-      </c>
-      <c r="AB65" s="10">
-        <v>1439.11</v>
-      </c>
-      <c r="AC65" s="10">
-        <v>1305.5</v>
-      </c>
-      <c r="AE65" s="10">
-        <v>1283.42</v>
-      </c>
-      <c r="AF65" s="10">
-        <v>1271.1300000000001</v>
-      </c>
-      <c r="AG65" s="10">
-        <v>1292.98</v>
-      </c>
-      <c r="AI65" s="10">
-        <v>1519.66</v>
-      </c>
-      <c r="AJ65" s="10">
-        <v>1537.73</v>
-      </c>
-      <c r="AK65" s="10">
-        <v>1530.58</v>
-      </c>
-    </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10"/>
-      <c r="O66" s="10"/>
-      <c r="P66" s="10"/>
-      <c r="Q66" s="10"/>
-      <c r="R66" s="10"/>
-      <c r="S66" s="10"/>
-      <c r="T66" s="10"/>
-      <c r="U66" s="10"/>
-      <c r="V66" s="10">
-        <v>0</v>
-      </c>
-      <c r="W66" s="10">
-        <v>0</v>
-      </c>
-      <c r="X66" s="10">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="10">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AA66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AB66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AF66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AG66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="9"/>
-      <c r="AI66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ66" s="10">
-        <v>0</v>
-      </c>
-      <c r="AK66" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="10"/>
@@ -3878,56 +4097,58 @@
       <c r="T67" s="10"/>
       <c r="U67" s="10"/>
       <c r="V67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="W67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="X67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Y67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="Z67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AA67" s="10">
-        <v>18.582899999999999</v>
+        <v>12</v>
       </c>
       <c r="AB67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AC67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AF67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AG67" s="10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AI67" s="10">
-        <v>0</v>
-      </c>
-      <c r="AJ67" s="10">
-        <v>42.2211</v>
-      </c>
-      <c r="AK67" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>8</v>
-      </c>
-      <c r="D68" s="10"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
-      <c r="G68" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="D68" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E68" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F68" s="10">
+        <v>10000</v>
+      </c>
+      <c r="G68" s="10">
+        <v>10000</v>
+      </c>
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
       <c r="J68" s="10"/>
@@ -3943,56 +4164,64 @@
       <c r="T68" s="10"/>
       <c r="U68" s="10"/>
       <c r="V68" s="10">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="W68" s="10">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="X68" s="10">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="Y68" s="10">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="Z68" s="10">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="AA68" s="10">
-        <v>170.00899999999999</v>
+        <v>10000</v>
       </c>
       <c r="AB68" s="10">
-        <v>17.891200000000001</v>
+        <v>5325</v>
       </c>
       <c r="AC68" s="10">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AE68" s="10">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="AF68" s="10">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="AG68" s="10">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AI68" s="10">
-        <v>781.649</v>
+        <v>1</v>
       </c>
       <c r="AJ68" s="10">
-        <v>609.85299999999995</v>
+        <v>10</v>
       </c>
       <c r="AK68" s="10">
-        <v>10.484</v>
-      </c>
-    </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="D69" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E69" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F69" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G69" s="10">
+        <v>0.5</v>
+      </c>
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
@@ -4008,56 +4237,52 @@
       <c r="T69" s="10"/>
       <c r="U69" s="10"/>
       <c r="V69" s="10">
-        <v>1286.48</v>
+        <v>20</v>
       </c>
       <c r="W69" s="10">
-        <v>1286.48</v>
+        <v>20</v>
       </c>
       <c r="X69" s="10">
-        <v>1280.43</v>
-      </c>
-      <c r="Y69" s="10">
-        <v>1300.27</v>
-      </c>
-      <c r="Z69" s="10">
-        <v>1296.97</v>
-      </c>
-      <c r="AA69" s="10">
-        <v>1588.37</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="Y69" s="10"/>
+      <c r="Z69" s="10"/>
+      <c r="AA69" s="10"/>
       <c r="AB69" s="10">
-        <v>1365.17</v>
-      </c>
-      <c r="AC69" s="10">
-        <v>1301.79</v>
+        <v>31</v>
+      </c>
+      <c r="AC69">
+        <v>53</v>
       </c>
       <c r="AE69" s="10">
-        <v>1266.6099999999999</v>
+        <v>38</v>
       </c>
       <c r="AF69" s="10">
-        <v>1266.6600000000001</v>
+        <v>39</v>
       </c>
       <c r="AG69" s="10">
-        <v>1277.4100000000001</v>
+        <v>38</v>
       </c>
       <c r="AI69" s="10">
-        <v>2301.31</v>
-      </c>
-      <c r="AJ69" s="10">
-        <v>2198.8000000000002</v>
-      </c>
-      <c r="AK69" s="10">
-        <v>1446.47</v>
-      </c>
-    </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="D70" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E70" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F70" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G70" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="10"/>
@@ -4072,74 +4297,1678 @@
       <c r="S70" s="10"/>
       <c r="T70" s="10"/>
       <c r="U70" s="10"/>
-      <c r="V70" s="10"/>
-      <c r="W70" s="10"/>
-      <c r="X70" s="10"/>
-      <c r="Y70" s="10">
+      <c r="V70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="W70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="X70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA70" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC70" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE70" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF70" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG70" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" s="8">
+        <v>1253.23</v>
+      </c>
+      <c r="D71" s="10">
+        <v>0</v>
+      </c>
+      <c r="E71" s="10">
+        <v>0</v>
+      </c>
+      <c r="F71" s="10">
+        <v>0</v>
+      </c>
+      <c r="G71" s="10">
+        <v>0</v>
+      </c>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+      <c r="O71" s="10"/>
+      <c r="P71" s="12"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10"/>
+      <c r="U71" s="12"/>
+      <c r="V71" s="12">
+        <v>1286.48</v>
+      </c>
+      <c r="W71" s="10">
+        <v>1286.48</v>
+      </c>
+      <c r="X71" s="10">
+        <v>1286.48</v>
+      </c>
+      <c r="Y71" s="10">
+        <v>1314.56</v>
+      </c>
+      <c r="Z71" s="10">
+        <v>1314.56</v>
+      </c>
+      <c r="AA71" s="10">
+        <v>1433.36</v>
+      </c>
+      <c r="AB71" s="10">
+        <v>1439.11</v>
+      </c>
+      <c r="AC71" s="10">
+        <v>1305.5</v>
+      </c>
+      <c r="AE71" s="10">
+        <v>1283.42</v>
+      </c>
+      <c r="AF71" s="10">
+        <v>1271.1300000000001</v>
+      </c>
+      <c r="AG71" s="10">
+        <v>1292.98</v>
+      </c>
+      <c r="AI71" s="10">
+        <v>1519.66</v>
+      </c>
+      <c r="AJ71" s="10">
+        <v>1537.73</v>
+      </c>
+      <c r="AK71" s="10">
+        <v>1530.58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" s="10">
+        <v>15</v>
+      </c>
+      <c r="E72" s="10">
+        <v>15</v>
+      </c>
+      <c r="F72" s="10">
+        <v>30</v>
+      </c>
+      <c r="G72" s="10">
+        <v>30</v>
+      </c>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+      <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
+      <c r="U72" s="10"/>
+      <c r="V72" s="10">
+        <v>0</v>
+      </c>
+      <c r="W72" s="10">
+        <v>0</v>
+      </c>
+      <c r="X72" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="9"/>
+      <c r="AI72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK72" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="10">
+        <v>1291.3699999999999</v>
+      </c>
+      <c r="E73" s="10">
+        <v>1291.3699999999999</v>
+      </c>
+      <c r="F73" s="10">
+        <v>1354.32</v>
+      </c>
+      <c r="G73" s="10">
+        <v>1354.32</v>
+      </c>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+      <c r="O73" s="10"/>
+      <c r="P73" s="10"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="10"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="10"/>
+      <c r="U73" s="10"/>
+      <c r="V73" s="10">
+        <v>0</v>
+      </c>
+      <c r="W73" s="10">
+        <v>0</v>
+      </c>
+      <c r="X73" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA73" s="10">
+        <v>18.582899999999999</v>
+      </c>
+      <c r="AB73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI73" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ73" s="10">
+        <v>42.2211</v>
+      </c>
+      <c r="AK73" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="10">
+        <v>0</v>
+      </c>
+      <c r="E74" s="10">
+        <v>0</v>
+      </c>
+      <c r="F74" s="10">
+        <v>0</v>
+      </c>
+      <c r="G74" s="10">
+        <v>0</v>
+      </c>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="10"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="10"/>
+      <c r="U74" s="10"/>
+      <c r="V74" s="10">
+        <v>0</v>
+      </c>
+      <c r="W74" s="10">
+        <v>0</v>
+      </c>
+      <c r="X74" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA74" s="10">
+        <v>170.00899999999999</v>
+      </c>
+      <c r="AB74" s="10">
+        <v>17.891200000000001</v>
+      </c>
+      <c r="AC74" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE74" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG74" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI74" s="10">
+        <v>781.649</v>
+      </c>
+      <c r="AJ74" s="10">
+        <v>609.85299999999995</v>
+      </c>
+      <c r="AK74" s="10">
+        <v>10.484</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="10">
+        <v>0</v>
+      </c>
+      <c r="E75" s="10">
+        <v>0</v>
+      </c>
+      <c r="F75" s="10">
+        <v>0</v>
+      </c>
+      <c r="G75" s="10">
+        <v>0</v>
+      </c>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+      <c r="O75" s="10"/>
+      <c r="P75" s="10"/>
+      <c r="Q75" s="10"/>
+      <c r="R75" s="10"/>
+      <c r="S75" s="10"/>
+      <c r="T75" s="10"/>
+      <c r="U75" s="10"/>
+      <c r="V75" s="10">
+        <v>1286.48</v>
+      </c>
+      <c r="W75" s="10">
+        <v>1286.48</v>
+      </c>
+      <c r="X75" s="10">
+        <v>1280.43</v>
+      </c>
+      <c r="Y75" s="10">
+        <v>1300.27</v>
+      </c>
+      <c r="Z75" s="10">
+        <v>1296.97</v>
+      </c>
+      <c r="AA75" s="10">
+        <v>1588.37</v>
+      </c>
+      <c r="AB75" s="10">
+        <v>1365.17</v>
+      </c>
+      <c r="AC75" s="10">
+        <v>1301.79</v>
+      </c>
+      <c r="AE75" s="10">
+        <v>1266.6099999999999</v>
+      </c>
+      <c r="AF75" s="10">
+        <v>1266.6600000000001</v>
+      </c>
+      <c r="AG75" s="10">
+        <v>1277.4100000000001</v>
+      </c>
+      <c r="AI75" s="10">
+        <v>2301.31</v>
+      </c>
+      <c r="AJ75" s="10">
+        <v>2198.8000000000002</v>
+      </c>
+      <c r="AK75" s="10">
+        <v>1446.47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="10">
+        <v>0</v>
+      </c>
+      <c r="E76" s="10">
+        <v>0</v>
+      </c>
+      <c r="F76" s="10">
+        <v>0</v>
+      </c>
+      <c r="G76" s="10">
+        <v>0</v>
+      </c>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+      <c r="O76" s="10"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="10"/>
+      <c r="R76" s="10"/>
+      <c r="S76" s="10"/>
+      <c r="T76" s="10"/>
+      <c r="U76" s="10"/>
+      <c r="V76" s="10"/>
+      <c r="W76" s="10"/>
+      <c r="X76" s="10"/>
+      <c r="Y76" s="10">
         <v>732</v>
       </c>
-      <c r="Z70" s="10">
+      <c r="Z76" s="10">
         <v>1926</v>
       </c>
-      <c r="AA70" s="10">
+      <c r="AA76" s="10">
         <v>1554</v>
       </c>
-      <c r="AB70" s="10">
+      <c r="AB76" s="10">
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
-    </row>
-    <row r="86" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J86" s="10"/>
-      <c r="K86" s="10"/>
-      <c r="L86" s="10"/>
-    </row>
-    <row r="87" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J87" s="10"/>
-      <c r="K87" s="10"/>
-      <c r="L87" s="10"/>
-    </row>
-    <row r="88" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J88" s="10"/>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-    </row>
-    <row r="89" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J89" s="10"/>
-      <c r="K89" s="10"/>
-      <c r="L89" s="10"/>
-    </row>
-    <row r="90" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J90" s="10"/>
-      <c r="K90" s="10"/>
-      <c r="L90" s="10"/>
-    </row>
-    <row r="91" spans="10:13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="10">
+        <v>0</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0</v>
+      </c>
+      <c r="F77" s="10">
+        <v>0</v>
+      </c>
+      <c r="G77" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C89"/>
+    </row>
+    <row r="90" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C90"/>
+    </row>
+    <row r="91" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C91"/>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
       <c r="L91" s="10"/>
     </row>
-    <row r="92" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="10:13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C92"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+    </row>
+    <row r="93" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C93"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+    </row>
+    <row r="94" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+    </row>
+    <row r="95" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C95"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+    </row>
+    <row r="96" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C96"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+    </row>
+    <row r="97" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C97"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+    </row>
+    <row r="98" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C98"/>
+    </row>
+    <row r="99" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C99"/>
+    </row>
+    <row r="100" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C100"/>
+    </row>
+    <row r="101" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C101"/>
+    </row>
+    <row r="102" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C102"/>
+    </row>
+    <row r="103" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C103"/>
+    </row>
+    <row r="104" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C104"/>
+    </row>
+    <row r="105" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C105"/>
+    </row>
+    <row r="106" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C106"/>
+    </row>
+    <row r="107" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C107"/>
+    </row>
+    <row r="108" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C108"/>
+    </row>
+    <row r="109" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C109"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:W43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="2:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C4" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H4" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="10">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10">
+        <v>15</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10">
+        <v>15</v>
+      </c>
+      <c r="H5" s="10">
+        <v>15</v>
+      </c>
+      <c r="I5" s="10">
+        <v>15</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C6" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="H6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2000</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C7" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="10">
+        <v>30000</v>
+      </c>
+      <c r="G7" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="10">
+        <v>20000</v>
+      </c>
+      <c r="I7" s="10">
+        <v>30000</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="10">
+        <v>19</v>
+      </c>
+      <c r="E9" s="10">
+        <v>19</v>
+      </c>
+      <c r="G9" s="10">
+        <v>19</v>
+      </c>
+      <c r="H9" s="10">
+        <v>19</v>
+      </c>
+      <c r="I9" s="10">
+        <v>19</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C10" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1723.18</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1723.18</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1714.99</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1712.84</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1706.93</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="10">
+        <v>17</v>
+      </c>
+      <c r="E13" s="10">
+        <v>17</v>
+      </c>
+      <c r="F13" s="10">
+        <v>17</v>
+      </c>
+      <c r="G13" s="10">
+        <v>17</v>
+      </c>
+      <c r="H13" s="10">
+        <v>17</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C14" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1536.81</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1536.81</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1527.24</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1531.2</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1531.2</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C18" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C22" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C26" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+      <c r="W28" s="10"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B29" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+      <c r="W29" s="10"/>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C30" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+      <c r="W30" s="10"/>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+    </row>
+    <row r="33" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+    </row>
+    <row r="34" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+    </row>
+    <row r="35" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+    </row>
+    <row r="36" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="10"/>
+    </row>
+    <row r="37" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+    </row>
+    <row r="38" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+    </row>
+    <row r="39" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+    </row>
+    <row r="40" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+    </row>
+    <row r="41" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+    </row>
+    <row r="42" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
+      <c r="W42" s="10"/>
+    </row>
+    <row r="43" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
+      <c r="W43" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8786,8 +10615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK103"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="T78" sqref="T78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>